<commit_message>
added role to users list
</commit_message>
<xml_diff>
--- a/employee_list.xlsx
+++ b/employee_list.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="従業員" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="部署" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="役職" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="従業員" sheetId="1" r:id="rId3" state="visible"/>
+    <sheet name="部署" sheetId="2" r:id="rId4" state="visible"/>
+    <sheet name="役職" sheetId="3" r:id="rId5" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">社員番号</t>
   </si>
@@ -52,12 +52,78 @@
   </si>
   <si>
     <t xml:space="preserve">メールアドレス</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>MAMBETLEPESOV</t>
+  </si>
+  <si>
+    <t>RINAT</t>
+  </si>
+  <si>
+    <t>Alik</t>
+  </si>
+  <si>
+    <t>EMPLOYEE</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>営業部</t>
+  </si>
+  <si>
+    <t>開発部</t>
+  </si>
+  <si>
+    <t>321321</t>
+  </si>
+  <si>
+    <t>rinatmambetlepesov@gmail.com</t>
+  </si>
+  <si>
+    <t>DK0002</t>
+  </si>
+  <si>
+    <t>dsadasdsad</t>
+  </si>
+  <si>
+    <t>sasadsa</t>
+  </si>
+  <si>
+    <t>dsadsa</t>
+  </si>
+  <si>
+    <t>justcheckout08@gmail.com</t>
+  </si>
+  <si>
+    <t>dsas</t>
+  </si>
+  <si>
+    <t>DK0001</t>
+  </si>
+  <si>
+    <t>Alikaa</t>
+  </si>
+  <si>
+    <t>rinatmambetlepeso@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin02</t>
+  </si>
+  <si>
+    <t>939207055</t>
+  </si>
+  <si>
+    <t>sarvarbekfozilov59@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
@@ -85,7 +151,7 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
@@ -93,7 +159,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b val="1"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK JP"/>
@@ -122,7 +188,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b val="1"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Noto Sans CJK SC"/>
@@ -172,14 +238,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -189,8 +255,8 @@
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -214,64 +280,64 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="right" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="right" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="left" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -388,14 +454,14 @@
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial" pitchFamily="0"/>
+        <a:ea typeface="Arial" pitchFamily="0"/>
+        <a:cs typeface="Arial" pitchFamily="0"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial" pitchFamily="0"/>
+        <a:ea typeface="Arial" pitchFamily="0"/>
+        <a:cs typeface="Arial" pitchFamily="0"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -514,30 +580,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:K4"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="1" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="12.63"/>
+    <col customWidth="true" max="1" min="1" style="1" width="13.75"/>
+    <col customWidth="true" max="6" min="2" style="1" width="12.63"/>
+    <col customWidth="true" max="7" min="7" style="1" width="20.44"/>
+    <col customWidth="true" max="8" min="8" style="1" width="17.38"/>
+    <col customWidth="true" max="10" min="9" style="1" width="12.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="17.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -569,51 +637,135 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" ht="12.8">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" ht="12.8">
+      <c r="A3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" ht="12.8">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="12.8">
+      <c r="A5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" ht="12.8">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -624,7 +776,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" ht="12.8">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -635,7 +787,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" ht="12.8">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -646,7 +798,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" ht="12.8">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -657,7 +809,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" ht="12.8">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -668,7 +820,7 @@
       <c r="I10" s="10"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" ht="12.8">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -679,7 +831,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" ht="12.8">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -690,7 +842,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" ht="12.8">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -701,7 +853,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" ht="12.8">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -712,7 +864,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" ht="12.8">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -723,7 +875,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" ht="12.8">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -734,7 +886,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" ht="12.8">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -745,7 +897,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" ht="12.8">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -756,7 +908,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" ht="12.8">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -767,7 +919,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" ht="12.8">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -778,7 +930,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" ht="12.8">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -789,7 +941,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" ht="12.8">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -800,7 +952,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" ht="12.8">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -811,7 +963,7 @@
       <c r="I23" s="10"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" ht="12.8">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -822,7 +974,7 @@
       <c r="I24" s="10"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" ht="12.8">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -833,7 +985,7 @@
       <c r="I25" s="10"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" ht="12.8">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -844,7 +996,7 @@
       <c r="I26" s="10"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" ht="12.8">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -855,7 +1007,7 @@
       <c r="I27" s="10"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" ht="12.8">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -866,7 +1018,7 @@
       <c r="I28" s="10"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" ht="12.8">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -877,7 +1029,7 @@
       <c r="I29" s="10"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" ht="12.8">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -888,7 +1040,7 @@
       <c r="I30" s="10"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" ht="12.8">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -899,7 +1051,7 @@
       <c r="I31" s="10"/>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" ht="12.8">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -910,7 +1062,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" ht="12.8">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -921,7 +1073,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" ht="12.8">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -932,7 +1084,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" ht="12.8">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -943,7 +1095,7 @@
       <c r="I35" s="10"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" ht="12.8">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -954,7 +1106,7 @@
       <c r="I36" s="10"/>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" ht="12.8">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -965,7 +1117,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" ht="12.8">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -976,7 +1128,7 @@
       <c r="I38" s="10"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" ht="12.8">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -987,7 +1139,7 @@
       <c r="I39" s="10"/>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" ht="12.8">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -998,7 +1150,7 @@
       <c r="I40" s="10"/>
       <c r="J40" s="7"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" ht="12.8">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1009,7 +1161,7 @@
       <c r="I41" s="10"/>
       <c r="J41" s="7"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" ht="12.8">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1020,7 +1172,7 @@
       <c r="I42" s="10"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" ht="12.8">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1031,7 +1183,7 @@
       <c r="I43" s="10"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" ht="12.8">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1042,7 +1194,7 @@
       <c r="I44" s="10"/>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" ht="12.8">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1053,7 +1205,7 @@
       <c r="I45" s="10"/>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" ht="12.8">
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1064,7 +1216,7 @@
       <c r="I46" s="10"/>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" ht="12.8">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1075,7 +1227,7 @@
       <c r="I47" s="10"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" ht="12.8">
       <c r="A48" s="6"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1086,7 +1238,7 @@
       <c r="I48" s="10"/>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" ht="12.8">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1097,7 +1249,7 @@
       <c r="I49" s="10"/>
       <c r="J49" s="7"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" ht="12.8">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1108,7 +1260,7 @@
       <c r="I50" s="10"/>
       <c r="J50" s="7"/>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" ht="12.8">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1119,7 +1271,7 @@
       <c r="I51" s="10"/>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" ht="12.8">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1130,7 +1282,7 @@
       <c r="I52" s="10"/>
       <c r="J52" s="7"/>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" ht="12.8">
       <c r="A53" s="6"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1141,7 +1293,7 @@
       <c r="I53" s="10"/>
       <c r="J53" s="7"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" ht="12.8">
       <c r="A54" s="6"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1152,7 +1304,7 @@
       <c r="I54" s="10"/>
       <c r="J54" s="7"/>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" ht="12.8">
       <c r="A55" s="6"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1163,7 +1315,7 @@
       <c r="I55" s="10"/>
       <c r="J55" s="7"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" ht="12.8">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1174,7 +1326,7 @@
       <c r="I56" s="10"/>
       <c r="J56" s="7"/>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" ht="12.8">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1185,7 +1337,7 @@
       <c r="I57" s="10"/>
       <c r="J57" s="7"/>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" ht="12.8">
       <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1196,7 +1348,7 @@
       <c r="I58" s="10"/>
       <c r="J58" s="7"/>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" ht="12.8">
       <c r="A59" s="6"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1207,7 +1359,7 @@
       <c r="I59" s="10"/>
       <c r="J59" s="7"/>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" ht="12.8">
       <c r="A60" s="6"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1218,7 +1370,7 @@
       <c r="I60" s="10"/>
       <c r="J60" s="7"/>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" ht="12.8">
       <c r="A61" s="6"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1229,7 +1381,7 @@
       <c r="I61" s="10"/>
       <c r="J61" s="7"/>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" ht="12.8">
       <c r="A62" s="6"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1240,7 +1392,7 @@
       <c r="I62" s="10"/>
       <c r="J62" s="7"/>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" ht="12.8">
       <c r="A63" s="6"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1251,7 +1403,7 @@
       <c r="I63" s="10"/>
       <c r="J63" s="7"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" ht="12.8">
       <c r="A64" s="6"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1262,7 +1414,7 @@
       <c r="I64" s="10"/>
       <c r="J64" s="7"/>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" ht="12.8">
       <c r="A65" s="6"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1273,7 +1425,7 @@
       <c r="I65" s="10"/>
       <c r="J65" s="7"/>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" ht="12.8">
       <c r="A66" s="6"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1284,7 +1436,7 @@
       <c r="I66" s="10"/>
       <c r="J66" s="7"/>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" ht="12.8">
       <c r="A67" s="6"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1295,7 +1447,7 @@
       <c r="I67" s="10"/>
       <c r="J67" s="7"/>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" ht="12.8">
       <c r="A68" s="6"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1306,7 +1458,7 @@
       <c r="I68" s="10"/>
       <c r="J68" s="7"/>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" ht="12.8">
       <c r="A69" s="6"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1317,7 +1469,7 @@
       <c r="I69" s="10"/>
       <c r="J69" s="7"/>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" ht="12.8">
       <c r="A70" s="6"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1328,7 +1480,7 @@
       <c r="I70" s="10"/>
       <c r="J70" s="7"/>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" ht="12.8">
       <c r="A71" s="6"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1339,7 +1491,7 @@
       <c r="I71" s="10"/>
       <c r="J71" s="7"/>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" ht="12.8">
       <c r="A72" s="6"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1350,7 +1502,7 @@
       <c r="I72" s="10"/>
       <c r="J72" s="7"/>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" ht="12.8">
       <c r="A73" s="6"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1361,7 +1513,7 @@
       <c r="I73" s="10"/>
       <c r="J73" s="7"/>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" ht="12.8">
       <c r="A74" s="6"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1372,7 +1524,7 @@
       <c r="I74" s="10"/>
       <c r="J74" s="7"/>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" ht="12.8">
       <c r="A75" s="6"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1383,7 +1535,7 @@
       <c r="I75" s="10"/>
       <c r="J75" s="7"/>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" ht="12.8">
       <c r="A76" s="6"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1394,7 +1546,7 @@
       <c r="I76" s="10"/>
       <c r="J76" s="7"/>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" ht="12.8">
       <c r="A77" s="6"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1405,7 +1557,7 @@
       <c r="I77" s="10"/>
       <c r="J77" s="7"/>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" ht="12.8">
       <c r="A78" s="6"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1416,7 +1568,7 @@
       <c r="I78" s="10"/>
       <c r="J78" s="7"/>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" ht="12.8">
       <c r="A79" s="6"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1427,7 +1579,7 @@
       <c r="I79" s="10"/>
       <c r="J79" s="7"/>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" ht="12.8">
       <c r="A80" s="6"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1438,7 +1590,7 @@
       <c r="I80" s="10"/>
       <c r="J80" s="7"/>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" ht="12.8">
       <c r="A81" s="6"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1449,7 +1601,7 @@
       <c r="I81" s="10"/>
       <c r="J81" s="7"/>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" ht="12.8">
       <c r="A82" s="6"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1460,7 +1612,7 @@
       <c r="I82" s="10"/>
       <c r="J82" s="7"/>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" ht="12.8">
       <c r="A83" s="6"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1471,7 +1623,7 @@
       <c r="I83" s="10"/>
       <c r="J83" s="7"/>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" ht="12.8">
       <c r="A84" s="6"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1482,7 +1634,7 @@
       <c r="I84" s="10"/>
       <c r="J84" s="7"/>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" ht="12.8">
       <c r="A85" s="6"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1493,7 +1645,7 @@
       <c r="I85" s="10"/>
       <c r="J85" s="7"/>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" ht="12.8">
       <c r="A86" s="6"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1504,7 +1656,7 @@
       <c r="I86" s="10"/>
       <c r="J86" s="7"/>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" ht="12.8">
       <c r="A87" s="6"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1515,7 +1667,7 @@
       <c r="I87" s="10"/>
       <c r="J87" s="7"/>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" ht="12.8">
       <c r="A88" s="6"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1526,7 +1678,7 @@
       <c r="I88" s="10"/>
       <c r="J88" s="7"/>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" ht="12.8">
       <c r="A89" s="6"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1537,7 +1689,7 @@
       <c r="I89" s="10"/>
       <c r="J89" s="7"/>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" ht="12.8">
       <c r="A90" s="6"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1548,7 +1700,7 @@
       <c r="I90" s="10"/>
       <c r="J90" s="7"/>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" ht="12.8">
       <c r="A91" s="6"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1559,7 +1711,7 @@
       <c r="I91" s="10"/>
       <c r="J91" s="7"/>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" ht="12.8">
       <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1570,7 +1722,7 @@
       <c r="I92" s="10"/>
       <c r="J92" s="7"/>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" ht="12.8">
       <c r="A93" s="6"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1581,7 +1733,7 @@
       <c r="I93" s="10"/>
       <c r="J93" s="7"/>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" ht="12.8">
       <c r="A94" s="6"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1592,7 +1744,7 @@
       <c r="I94" s="10"/>
       <c r="J94" s="7"/>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" ht="12.8">
       <c r="A95" s="6"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1603,7 +1755,7 @@
       <c r="I95" s="10"/>
       <c r="J95" s="7"/>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" ht="12.8">
       <c r="A96" s="6"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1614,7 +1766,7 @@
       <c r="I96" s="10"/>
       <c r="J96" s="7"/>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" ht="12.8">
       <c r="A97" s="6"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1625,7 +1777,7 @@
       <c r="I97" s="10"/>
       <c r="J97" s="7"/>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" ht="12.8">
       <c r="A98" s="6"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1636,7 +1788,7 @@
       <c r="I98" s="10"/>
       <c r="J98" s="7"/>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" ht="12.8">
       <c r="A99" s="6"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1647,7 +1799,7 @@
       <c r="I99" s="10"/>
       <c r="J99" s="7"/>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" ht="12.8">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1658,7 +1810,7 @@
       <c r="I100" s="10"/>
       <c r="J100" s="7"/>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" ht="12.8">
       <c r="A101" s="6"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1671,157 +1823,152 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G101" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showErrorMessage="true" sqref="G2:G101" type="list">
       <formula1>部署!$A$2:$A1000</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H101" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showErrorMessage="true" sqref="H2:H101" type="list">
       <formula1>役職!$A$2:$A1000</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLinesSet="true"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:K4"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
+    <col customWidth="true" max="3" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="15">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" ht="13.8">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" ht="13.8">
       <c r="A3" s="12"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" ht="13.8">
       <c r="A4" s="12"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" ht="15.75" customHeight="true">
       <c r="A5" s="13"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="15.75" customHeight="true">
       <c r="A6" s="13"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" ht="15.75" customHeight="true">
       <c r="A7" s="13"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" ht="15.75" customHeight="true">
       <c r="A8" s="13"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" ht="15.75" customHeight="true">
       <c r="A9" s="13"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" ht="15.75" customHeight="true">
       <c r="A10" s="13"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" ht="15.75" customHeight="true">
       <c r="A11" s="13"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" ht="15.75" customHeight="true">
       <c r="A12" s="13"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" ht="15.75" customHeight="true">
       <c r="A13" s="13"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" ht="15.75" customHeight="true">
       <c r="A14" s="13"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLinesSet="true"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:K4"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
+    <col customWidth="true" max="3" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="15">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" ht="13.8">
+      <c r="A2" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" ht="12.8">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" ht="12.8">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" ht="15.75" customHeight="true">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="15.75" customHeight="true">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" ht="15.75" customHeight="true">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" ht="15.75" customHeight="true">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" ht="15.75" customHeight="true">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" ht="15.75" customHeight="true">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" ht="15.75" customHeight="true">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" ht="15.75" customHeight="true">
       <c r="A12" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLinesSet="true"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added google sign-in func
</commit_message>
<xml_diff>
--- a/employee_list.xlsx
+++ b/employee_list.xlsx
@@ -671,7 +671,7 @@
     </row>
     <row r="3" ht="12.8">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>11</v>
@@ -680,7 +680,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>14</v>
@@ -695,10 +695,10 @@
         <v>17</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="12.8">

</xml_diff>